<commit_message>
Comparing old data and Race 1.0 in new data
</commit_message>
<xml_diff>
--- a/Phase_2/results.xlsx
+++ b/Phase_2/results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shour\OneDrive\Desktop\GxE_Analysis\Phase_2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shouryamaheshwari/Desktop/GxE-Study/Phase_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3941361D-9BAA-416B-B6ED-DF55F78CA4B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE80271B-6D24-9545-92F0-D4DD324E0327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="With_TL_AST" sheetId="1" r:id="rId1"/>
@@ -107,7 +107,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="168" formatCode="0.00000"/>
+    <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -212,47 +212,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -265,36 +252,31 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -581,303 +563,303 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J5" sqref="J5"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="15.77734375" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="15.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.88671875" style="3"/>
+    <col min="13" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="7" t="s">
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.3">
-      <c r="A2" s="11"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="14" t="s">
+    <row r="2" spans="1:12" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.2">
+      <c r="A2" s="7"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
-      <c r="K2" s="36"/>
-      <c r="L2" s="36"/>
-    </row>
-    <row r="3" spans="1:12" ht="18" x14ac:dyDescent="0.3">
-      <c r="A3" s="16">
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+    </row>
+    <row r="3" spans="1:12" ht="19" x14ac:dyDescent="0.2">
+      <c r="A3" s="11">
         <v>0.79646017699115002</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="18" t="s">
+      <c r="C3" s="8"/>
+      <c r="D3" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="19">
+      <c r="E3" s="14">
         <v>0.805755395683453</v>
       </c>
-      <c r="F3" s="19">
+      <c r="F3" s="14">
         <v>0.75265957446808496</v>
       </c>
-      <c r="G3" s="19">
+      <c r="G3" s="14">
         <v>0.80392156862745101</v>
       </c>
-      <c r="H3" s="19">
+      <c r="H3" s="14">
         <v>0.74774774774774699</v>
       </c>
-      <c r="I3" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="J3" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="K3" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="L3" s="11" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="144" x14ac:dyDescent="0.3">
-      <c r="A4" s="16">
+      <c r="I3" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="J3" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="K3" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="L3" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="160" x14ac:dyDescent="0.2">
+      <c r="A4" s="11">
         <v>0.80727740276438398</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="19">
+      <c r="E4" s="14">
         <v>0.80485611510791299</v>
       </c>
-      <c r="F4" s="19">
+      <c r="F4" s="14">
         <v>0.76063829787234005</v>
       </c>
-      <c r="G4" s="19">
+      <c r="G4" s="14">
         <v>0.80392156862745101</v>
       </c>
-      <c r="H4" s="19">
+      <c r="H4" s="14">
         <v>0.76576576576576505</v>
       </c>
-      <c r="I4" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="J4" s="37" t="b">
-        <v>1</v>
-      </c>
-      <c r="K4" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="L4" s="37" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="126" x14ac:dyDescent="0.3">
-      <c r="A5" s="16">
+      <c r="I4" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="J4" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="K4" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="L4" s="24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="140" x14ac:dyDescent="0.2">
+      <c r="A5" s="11">
         <v>0.80793314046930198</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="19">
+      <c r="E5" s="14">
         <v>0.80125899280575497</v>
       </c>
-      <c r="F5" s="19">
+      <c r="F5" s="14">
         <v>0.75531914893617003</v>
       </c>
-      <c r="G5" s="19">
+      <c r="G5" s="14">
         <v>0.80392156862745101</v>
       </c>
-      <c r="H5" s="19">
+      <c r="H5" s="14">
         <v>0.74774774774774699</v>
       </c>
-      <c r="I5" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="J5" s="37" t="b">
-        <v>1</v>
-      </c>
-      <c r="K5" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="L5" s="37" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="18" x14ac:dyDescent="0.3">
-      <c r="A6" s="16">
+      <c r="I5" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="J5" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="K5" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="L5" s="24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="19" x14ac:dyDescent="0.2">
+      <c r="A6" s="11">
         <v>0.80727740276438398</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="18" t="s">
+      <c r="C6" s="16"/>
+      <c r="D6" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="19">
+      <c r="E6" s="14">
         <v>0.80305755395683398</v>
       </c>
-      <c r="F6" s="19">
+      <c r="F6" s="14">
         <v>0.76063829787234005</v>
       </c>
-      <c r="G6" s="19">
+      <c r="G6" s="14">
         <v>0.80392156862745101</v>
       </c>
-      <c r="H6" s="19">
+      <c r="H6" s="14">
         <v>0.74774774774774699</v>
       </c>
-      <c r="I6" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="J6" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="K6" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="L6" s="37" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="18" x14ac:dyDescent="0.3">
-      <c r="A7" s="16">
+      <c r="I6" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="J6" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="K6" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="L6" s="24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="19" x14ac:dyDescent="0.2">
+      <c r="A7" s="11">
         <v>0.80105003750133896</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="12"/>
-      <c r="D7" s="17" t="s">
+      <c r="C7" s="8"/>
+      <c r="D7" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="14">
         <v>0.90107913669064699</v>
       </c>
-      <c r="F7" s="19">
+      <c r="F7" s="14">
         <v>0.76595744680850997</v>
       </c>
-      <c r="G7" s="19">
+      <c r="G7" s="14">
         <v>0.82352941176470495</v>
       </c>
-      <c r="H7" s="19">
+      <c r="H7" s="14">
         <v>0.74774774774774699</v>
       </c>
-      <c r="I7" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="J7" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="K7" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="L7" s="37" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="180" x14ac:dyDescent="0.3">
-      <c r="A8" s="11">
+      <c r="I7" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="J7" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="K7" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="L7" s="24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="180" x14ac:dyDescent="0.2">
+      <c r="A8" s="7">
         <v>0.80793206900246395</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="19">
+      <c r="E8" s="14">
         <v>0.82014388489208601</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="7">
         <v>0.75</v>
       </c>
-      <c r="G8" s="19">
+      <c r="G8" s="14">
         <v>0.80392156862745101</v>
       </c>
-      <c r="H8" s="19">
+      <c r="H8" s="14">
         <v>0.78378378378378299</v>
       </c>
-      <c r="I8" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="J8" s="37" t="b">
-        <v>1</v>
-      </c>
-      <c r="K8" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="L8" s="37" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C17" s="5"/>
+      <c r="I8" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="J8" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="K8" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="L8" s="24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C17" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -907,216 +889,216 @@
       <selection activeCell="G5" sqref="A1:L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.77734375" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.109375" style="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="8" style="20" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.44140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.109375" style="20" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.6640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.88671875" style="20"/>
+    <col min="1" max="1" width="23.83203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.1640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5" style="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.1640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.6640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.83203125" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="10" t="s">
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="K1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="L1" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2" s="11"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="14" t="s">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A3" s="16">
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="11">
         <v>0.323500491642084</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="18" t="s">
+      <c r="C3" s="8"/>
+      <c r="D3" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="19">
+      <c r="E3" s="14">
         <v>0.5</v>
       </c>
-      <c r="F3" s="19">
+      <c r="F3" s="14">
         <v>0.40495867768595001</v>
       </c>
-      <c r="G3" s="19">
+      <c r="G3" s="14">
         <v>0.5</v>
       </c>
-      <c r="H3" s="19">
+      <c r="H3" s="14">
         <v>0.42268041237113402</v>
       </c>
-      <c r="I3" s="22" t="b">
-        <v>1</v>
-      </c>
-      <c r="J3" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="K3" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="L3" s="20" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A4" s="16">
+      <c r="I3" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="K3" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="L3" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="11">
         <v>0.43657817109144498</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="18" t="s">
+      <c r="C4" s="16"/>
+      <c r="D4" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="19">
+      <c r="E4" s="14">
         <v>0.53163444639718804</v>
       </c>
-      <c r="F4" s="19">
+      <c r="F4" s="14">
         <v>0.413223140495867</v>
       </c>
-      <c r="G4" s="19">
+      <c r="G4" s="14">
         <v>0.5</v>
       </c>
-      <c r="H4" s="19">
+      <c r="H4" s="14">
         <v>0.42268041237113402</v>
       </c>
-      <c r="I4" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="J4" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="K4" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="L4" s="20" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A5" s="16"/>
-      <c r="B5" s="17" t="s">
+      <c r="I4" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J4" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="K4" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="L4" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="11"/>
+      <c r="B5" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="18" t="s">
+      <c r="C5" s="16"/>
+      <c r="D5" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A6" s="16"/>
-      <c r="B6" s="17" t="s">
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="11"/>
+      <c r="B6" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="18" t="s">
+      <c r="C6" s="16"/>
+      <c r="D6" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A7" s="16">
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="11">
         <v>0.56015536269152399</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="12"/>
-      <c r="D7" s="17" t="s">
+      <c r="C7" s="8"/>
+      <c r="D7" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="14">
         <v>0.57820738137082595</v>
       </c>
-      <c r="F7" s="19">
+      <c r="F7" s="14">
         <v>0.413223140495867</v>
       </c>
-      <c r="G7" s="19">
+      <c r="G7" s="14">
         <v>0.59615384615384603</v>
       </c>
-      <c r="H7" s="19">
+      <c r="H7" s="14">
         <v>0.49484536082474201</v>
       </c>
-      <c r="I7" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="J7" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="K7" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="L7" s="22" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B8" s="17" t="s">
+      <c r="I7" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J7" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="K7" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="L7" s="17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B8" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="21"/>
-      <c r="D8" s="17" t="s">
+      <c r="C8" s="16"/>
+      <c r="D8" s="12" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1149,136 +1131,135 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.21875" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="15.77734375" style="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.44140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.109375" style="20" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="20"/>
+    <col min="1" max="1" width="17.1640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.1640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="15.83203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5" style="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.83203125" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A1" s="34"/>
-      <c r="B1" s="34" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="22"/>
+      <c r="B1" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="35"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A2" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="25" t="s">
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="23"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="10" t="s">
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="15" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="26"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="27" t="s">
+    <row r="3" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="F3" s="18" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" s="28" t="s">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="29">
+      <c r="B4" s="18"/>
+      <c r="C4" s="20">
         <v>0.80665467625899201</v>
       </c>
-      <c r="D4" s="29">
+      <c r="D4" s="20">
         <v>0.76329787234042501</v>
       </c>
-      <c r="E4" s="29">
+      <c r="E4" s="20">
         <v>0.80392156862745101</v>
       </c>
-      <c r="F4" s="29">
+      <c r="F4" s="20">
         <v>0.76576576576576505</v>
       </c>
-      <c r="G4" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="H4" s="20" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A5" s="30" t="s">
+      <c r="G4" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="33"/>
-      <c r="C5" s="20">
+      <c r="C5" s="15">
         <v>0.80485611510791299</v>
       </c>
-      <c r="D5" s="20">
+      <c r="D5" s="15">
         <v>0.75265957446808496</v>
       </c>
-      <c r="E5" s="20">
+      <c r="E5" s="15">
         <v>0.74509803921568596</v>
       </c>
-      <c r="F5" s="20">
+      <c r="F5" s="15">
         <v>0.73873873873873797</v>
       </c>
-      <c r="G5" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="H5" s="20" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B6" s="15" t="s">
+      <c r="G5" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B6" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="20">
+      <c r="C6" s="15">
         <v>0.81205035971223005</v>
       </c>
-      <c r="D6" s="20">
+      <c r="D6" s="15">
         <v>0.76595744680850997</v>
       </c>
-      <c r="E6" s="20">
+      <c r="E6" s="15">
         <v>0.80392156862745101</v>
       </c>
-      <c r="F6" s="20">
+      <c r="F6" s="15">
         <v>0.76576576576576505</v>
       </c>
-      <c r="G6" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="H6" s="20" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="N9" s="8"/>
+      <c r="G6" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6" s="15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N9" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1298,159 +1279,159 @@
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.21875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="6" width="8" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="3"/>
+    <col min="7" max="7" width="13.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="24"/>
-      <c r="B1" s="24" t="s">
+    <row r="1" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A1" s="18"/>
+      <c r="B1" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-    </row>
-    <row r="2" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="25" t="s">
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+    </row>
+    <row r="2" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="10"/>
+      <c r="C2" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="10" t="s">
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A3" s="26"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="27" t="s">
+    <row r="3" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="F3" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-    </row>
-    <row r="4" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A4" s="28" t="s">
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+    </row>
+    <row r="4" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="29">
+      <c r="B4" s="18"/>
+      <c r="C4" s="20">
         <v>0.538664323374341</v>
       </c>
-      <c r="D4" s="29">
+      <c r="D4" s="20">
         <v>0.39393939393939298</v>
       </c>
-      <c r="E4" s="29">
+      <c r="E4" s="20">
         <v>0.63461538461538403</v>
       </c>
-      <c r="F4" s="29">
+      <c r="F4" s="20">
         <v>0.49484536082474201</v>
       </c>
-      <c r="G4" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="H4" s="20" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A5" s="28" t="s">
+      <c r="G4" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="29">
+      <c r="B5" s="18"/>
+      <c r="C5" s="20">
         <v>0.49121265377855799</v>
       </c>
-      <c r="D5" s="29">
+      <c r="D5" s="20">
         <v>0.443526170798898</v>
       </c>
-      <c r="E5" s="29">
+      <c r="E5" s="20">
         <v>0.63461538461538403</v>
       </c>
-      <c r="F5" s="29">
+      <c r="F5" s="20">
         <v>0.45360824742268002</v>
       </c>
-      <c r="G5" s="22" t="b">
-        <v>1</v>
-      </c>
-      <c r="H5" s="20" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A6" s="30" t="s">
+      <c r="G5" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A6" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="33"/>
-      <c r="C6" s="20">
+      <c r="B6" s="10"/>
+      <c r="C6" s="15">
         <v>0.54745166959578195</v>
       </c>
-      <c r="D6" s="20">
+      <c r="D6" s="15">
         <v>0.39393939393939298</v>
       </c>
-      <c r="E6" s="20">
+      <c r="E6" s="15">
         <v>0.42307692307692302</v>
       </c>
-      <c r="F6" s="20">
+      <c r="F6" s="15">
         <v>0.55670103092783496</v>
       </c>
-      <c r="G6" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="H6" s="20" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A7" s="30" t="s">
+      <c r="G6" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A7" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="20">
+      <c r="B7" s="10"/>
+      <c r="C7" s="15">
         <v>0.47891036906854101</v>
       </c>
-      <c r="D7" s="20">
+      <c r="D7" s="15">
         <v>0.38842975206611502</v>
       </c>
-      <c r="E7" s="20">
+      <c r="E7" s="15">
         <v>0.42307692307692302</v>
       </c>
-      <c r="F7" s="20">
+      <c r="F7" s="15">
         <v>0.432989690721649</v>
       </c>
-      <c r="G7" s="22" t="b">
-        <v>1</v>
-      </c>
-      <c r="H7" s="20" t="b">
+      <c r="G7" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" s="15" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updating RF_RF_v1 using cv
</commit_message>
<xml_diff>
--- a/Phase_2/results.xlsx
+++ b/Phase_2/results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shouryamaheshwari/Desktop/GxE-Study/Phase_2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shour\OneDrive\Desktop\GxE_Analysis\Phase_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE80271B-6D24-9545-92F0-D4DD324E0327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4566618-3859-4698-9F52-56250C2D481C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="With_TL_AST" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="22">
   <si>
     <t>Model Name</t>
   </si>
@@ -91,14 +91,10 @@
     <t>max_iter=3800, solver='saga', penalty='l2', C=0.03359818286283781,                                  multi_class='multinomial'</t>
   </si>
   <si>
-    <t>n_estimators=750, max_depth=80, random_state=42, min_samples_split=20,
-                                        min_samples_leaf=15, max_features='sqrt', bootstrap=True</t>
-  </si>
-  <si>
     <t>LightGBM</t>
   </si>
   <si>
-    <t>Best Parameters for final model (race 4.0): {'subsample': 0.9736842105263157, 'reg_lambda': 0.5555555555555556, 'reg_alpha': 0.8888888888888888, 'num_leaves': 315, 'min_split_gain': 0.4444444444444444, 'min_child_samples': 91, 'max_depth': 7, 'learning_rate': 0.007937005259840991, 'colsample_bytree': 0.7777777777777778}</t>
+    <t>Base Model Val Accuracy</t>
   </si>
 </sst>
 </file>
@@ -561,30 +557,28 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:L8"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="15.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.83203125" style="3"/>
+    <col min="1" max="1" width="28.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="8.21875" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.21875" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.77734375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>10</v>
@@ -614,7 +608,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -636,7 +630,7 @@
       <c r="K2" s="8"/>
       <c r="L2" s="8"/>
     </row>
-    <row r="3" spans="1:12" ht="19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" ht="18" x14ac:dyDescent="0.3">
       <c r="A3" s="11">
         <v>0.79646017699115002</v>
       </c>
@@ -672,7 +666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="160" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="144" x14ac:dyDescent="0.3">
       <c r="A4" s="11">
         <v>0.80727740276438398</v>
       </c>
@@ -710,7 +704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="140" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="126" x14ac:dyDescent="0.3">
       <c r="A5" s="11">
         <v>0.80793314046930198</v>
       </c>
@@ -748,7 +742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="19" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="18" x14ac:dyDescent="0.3">
       <c r="A6" s="11">
         <v>0.80727740276438398</v>
       </c>
@@ -784,9 +778,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="19" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="18" x14ac:dyDescent="0.3">
       <c r="A7" s="11">
-        <v>0.80105003750133896</v>
+        <v>0.80727630285152396</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>6</v>
@@ -796,16 +790,16 @@
         <v>18</v>
       </c>
       <c r="E7" s="14">
-        <v>0.90107913669064699</v>
+        <v>0.82284172661870503</v>
       </c>
       <c r="F7" s="14">
-        <v>0.76595744680850997</v>
+        <v>0.75531914893617003</v>
       </c>
       <c r="G7" s="14">
         <v>0.82352941176470495</v>
       </c>
       <c r="H7" s="14">
-        <v>0.74774774774774699</v>
+        <v>0.76576576576576505</v>
       </c>
       <c r="I7" s="7" t="b">
         <v>0</v>
@@ -816,49 +810,45 @@
       <c r="K7" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="L7" s="24" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="180" x14ac:dyDescent="0.2">
-      <c r="A8" s="7">
-        <v>0.80793206900246395</v>
+      <c r="L7" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="18" x14ac:dyDescent="0.3">
+      <c r="A8" s="11">
+        <v>0.80793217246652804</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="16" t="s">
-        <v>20</v>
-      </c>
+      <c r="C8" s="8"/>
       <c r="D8" s="12" t="s">
         <v>18</v>
       </c>
       <c r="E8" s="14">
-        <v>0.82014388489208601</v>
-      </c>
-      <c r="F8" s="7">
-        <v>0.75</v>
+        <v>0.80570822143290299</v>
+      </c>
+      <c r="F8" s="14">
+        <v>0.77907545554604296</v>
       </c>
       <c r="G8" s="14">
-        <v>0.80392156862745101</v>
+        <v>0.79393939393939394</v>
       </c>
       <c r="H8" s="14">
-        <v>0.78378378378378299</v>
-      </c>
-      <c r="I8" s="7" t="b">
-        <v>0</v>
-      </c>
+        <v>0.83870129870129795</v>
+      </c>
+      <c r="I8" s="7"/>
       <c r="J8" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="K8" s="7" t="b">
-        <v>0</v>
+      <c r="K8" s="24" t="b">
+        <v>1</v>
       </c>
       <c r="L8" s="24" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C17" s="4"/>
     </row>
   </sheetData>
@@ -866,7 +856,7 @@
     <mergeCell ref="E1:H1"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:L8">
-    <cfRule type="colorScale" priority="1">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -886,24 +876,24 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="A1:L8"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.83203125" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.83203125" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.1640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5" style="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.77734375" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.77734375" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.44140625" style="15" bestFit="1" customWidth="1"/>
     <col min="5" max="8" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5" style="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.44140625" style="15" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.33203125" style="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.1640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.109375" style="15" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.6640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.83203125" style="15"/>
+    <col min="13" max="16384" width="8.77734375" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
@@ -935,7 +925,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -957,7 +947,7 @@
       <c r="K2" s="10"/>
       <c r="L2" s="10"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="11">
         <v>0.323500491642084</v>
       </c>
@@ -993,7 +983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="11">
         <v>0.43657817109144498</v>
       </c>
@@ -1029,7 +1019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="11"/>
       <c r="B5" s="12" t="s">
         <v>8</v>
@@ -1043,7 +1033,7 @@
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="11"/>
       <c r="B6" s="12" t="s">
         <v>8</v>
@@ -1057,7 +1047,7 @@
       <c r="G6" s="14"/>
       <c r="H6" s="14"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="11">
         <v>0.56015536269152399</v>
       </c>
@@ -1093,7 +1083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B8" s="12" t="s">
         <v>6</v>
       </c>
@@ -1127,21 +1117,21 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H6" activeCellId="1" sqref="C17 H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.1640625" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.1640625" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="15.83203125" style="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5" style="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.83203125" style="15"/>
+    <col min="1" max="1" width="17.109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="15.77734375" style="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.44140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.77734375" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="22"/>
       <c r="B1" s="22" t="s">
         <v>16</v>
@@ -1155,7 +1145,7 @@
       <c r="G1" s="22"/>
       <c r="H1" s="23"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
@@ -1172,7 +1162,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="18"/>
       <c r="B3" s="18"/>
       <c r="C3" s="18" t="s">
@@ -1188,33 +1178,33 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="19" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="18"/>
       <c r="C4" s="20">
-        <v>0.80665467625899201</v>
+        <v>0.803650264229403</v>
       </c>
       <c r="D4" s="20">
-        <v>0.76329787234042501</v>
+        <v>0.78088541029717495</v>
       </c>
       <c r="E4" s="20">
-        <v>0.80392156862745101</v>
+        <v>0.81212121212121202</v>
       </c>
       <c r="F4" s="20">
-        <v>0.76576576576576505</v>
+        <v>0.83870129870129795</v>
       </c>
       <c r="G4" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="H4" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H4" s="17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" s="15">
         <v>0.80485611510791299</v>
@@ -1235,30 +1225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="15">
-        <v>0.81205035971223005</v>
-      </c>
-      <c r="D6" s="15">
-        <v>0.76595744680850997</v>
-      </c>
-      <c r="E6" s="15">
-        <v>0.80392156862745101</v>
-      </c>
-      <c r="F6" s="15">
-        <v>0.76576576576576505</v>
-      </c>
-      <c r="G6" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H6" s="15" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="N9" s="5"/>
     </row>
   </sheetData>
@@ -1276,20 +1243,20 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.109375" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="6" width="8" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.83203125" style="3"/>
+    <col min="7" max="7" width="13.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.77734375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="18"/>
       <c r="B1" s="18" t="s">
         <v>16</v>
@@ -1303,7 +1270,7 @@
       <c r="G1" s="18"/>
       <c r="H1" s="18"/>
     </row>
-    <row r="2" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
@@ -1321,7 +1288,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="18"/>
       <c r="B3" s="18"/>
       <c r="C3" s="18" t="s">
@@ -1339,7 +1306,7 @@
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
     </row>
-    <row r="4" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A4" s="19" t="s">
         <v>6</v>
       </c>
@@ -1363,7 +1330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A5" s="19" t="s">
         <v>6</v>
       </c>
@@ -1387,9 +1354,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" s="10"/>
       <c r="C6" s="15">
@@ -1411,9 +1378,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A7" s="21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="15">

</xml_diff>